<commit_message>
Added dynamic messaging system
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excel Sheets/WinkelDiefstal.xlsx
+++ b/Assets/Resources/Excel Sheets/WinkelDiefstal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_BartVR\Assets\Resources\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D340C22-30BF-4539-918A-366CCF87E74F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0B5522-6749-4A1F-BAA1-2B26F7BBBD67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
+    <workbookView minimized="1" xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -176,15 +176,9 @@
     <t>Is de verdachte gevaarlijk?</t>
   </si>
   <si>
-    <t>Ik zag iemand hier wegrennen met een tas!</t>
-  </si>
-  <si>
     <t>Tas was hier gedumpt, heb het naar de politie gebracht.</t>
   </si>
   <si>
-    <t>Loop hij hier nog ergens rond?</t>
-  </si>
-  <si>
     <t>Is dit al opgelost?</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>Was de verdachte een vrouw?</t>
   </si>
   <si>
-    <t>De man rende hier gauw weg!</t>
-  </si>
-  <si>
     <t>Hoe ziet de verdachte eruit?</t>
   </si>
   <si>
@@ -305,10 +296,19 @@
     <t>Postable</t>
   </si>
   <si>
-    <t>Iemand heeft hier een mobiel uit mijn winkel gestolen</t>
-  </si>
-  <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>Een [geslacht] heeft hier een mobiel uit mijn winkel gestolen</t>
+  </si>
+  <si>
+    <t>De [geslacht] rende hier gauw weg!</t>
+  </si>
+  <si>
+    <t>Ik zag iemand hier wegrennen met een [bovenstuk] bovenstuk!</t>
+  </si>
+  <si>
+    <t>Loopt die persoon met het [onderstuk] onderstuk hier nog ergens rond?</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,20 +844,20 @@
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
     <col min="5" max="8" width="18.140625" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -869,19 +869,19 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
@@ -893,16 +893,16 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
@@ -916,16 +916,16 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
@@ -937,14 +937,14 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
@@ -956,14 +956,14 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -975,14 +975,14 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -995,7 +995,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
@@ -1014,7 +1014,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
@@ -1033,14 +1033,14 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
@@ -1052,14 +1052,14 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
@@ -1071,14 +1071,14 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
@@ -1090,16 +1090,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1111,14 +1111,14 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1130,14 +1130,14 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1149,14 +1149,14 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
@@ -1168,14 +1168,14 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1187,14 +1187,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
@@ -1206,14 +1206,14 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
@@ -1225,17 +1225,17 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>2</v>
@@ -1246,14 +1246,14 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
@@ -1267,16 +1267,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
@@ -1288,7 +1288,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
@@ -1309,14 +1309,14 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">

</xml_diff>